<commit_message>
Google Search Bar added
</commit_message>
<xml_diff>
--- a/Images/Countries.xlsx
+++ b/Images/Countries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zur Bonsen Georg\Documents\Programme\Beyond4P\B4P_Docu_Maker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zur-b\OneDrive\Documents\Programme\Beyond4P\B4P_Docu_Maker\"/>
       <!-- B4P: Insert the path name -->
     </mc:Choice>
   </mc:AlternateContent>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>Country name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Antigua and Barbuda</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
     <t>Benin</t>
   </si>
   <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
     <t>Botswana</t>
   </si>
   <si>
@@ -111,9 +111,6 @@
     <t>Chad</t>
   </si>
   <si>
-    <t>Chile</t>
-  </si>
-  <si>
     <t>China</t>
   </si>
   <si>
@@ -258,7 +255,7 @@
     <t>Mauritius</t>
   </si>
   <si>
-    <t>Mexico</t>
+    <t>Federated States of Micronesia</t>
   </si>
   <si>
     <t>Monaco</t>
@@ -385,9 +382,6 @@
   </si>
   <si>
     <t>Uganda</t>
-  </si>
-  <si>
-    <t>Uruguay</t>
   </si>
   <si>
     <t>Vanuatu</t>
@@ -777,7 +771,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0000-0000-0000-000000000000}">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H113"/>
   <!-- B4P: Example: A1:Z9 -->
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1" showGridLines="0">
@@ -838,7 +832,7 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
     </row>
@@ -847,12 +841,12 @@
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -874,7 +868,7 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="G6">
         <v>1</v>
       </c>
     </row>
@@ -882,7 +876,10 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="G7">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
     </row>
@@ -891,14 +888,12 @@
         <v>14</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -907,10 +902,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -920,7 +915,7 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1</v>
       </c>
     </row>
@@ -1024,7 +1019,7 @@
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="E19">
+      <c r="B19">
         <v>1</v>
       </c>
     </row>
@@ -1032,10 +1027,10 @@
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1060,7 +1055,7 @@
       <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="C22">
+      <c r="E22">
         <v>1</v>
       </c>
     </row>
@@ -1068,7 +1063,7 @@
       <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="E23">
+      <c r="D23">
         <v>1</v>
       </c>
     </row>
@@ -1104,7 +1099,7 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="D26">
+      <c r="C26">
         <v>1</v>
       </c>
     </row>
@@ -1112,7 +1107,7 @@
       <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="C27">
+      <c r="E27">
         <v>1</v>
       </c>
     </row>
@@ -1122,10 +1117,10 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2">
-        <v>1</v>
-      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1136,10 +1131,10 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1148,7 +1143,7 @@
       <c r="A30" t="s">
         <v>36</v>
       </c>
-      <c r="E30">
+      <c r="D30">
         <v>1</v>
       </c>
     </row>
@@ -1156,7 +1151,7 @@
       <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="D31">
+      <c r="C31">
         <v>1</v>
       </c>
     </row>
@@ -1165,11 +1160,11 @@
         <v>38</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
+      <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1200,6 +1195,9 @@
       <c r="A35" t="s">
         <v>41</v>
       </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
       <c r="E35">
         <v>1</v>
       </c>
@@ -1209,13 +1207,11 @@
         <v>42</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2">
-        <v>1</v>
-      </c>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1232,16 +1228,15 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="H38">
+      <c r="D38">
         <v>1</v>
       </c>
     </row>
@@ -1258,10 +1253,10 @@
         <v>46</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2">
-        <v>1</v>
-      </c>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1272,12 +1267,12 @@
         <v>47</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="2">
-        <v>1</v>
-      </c>
+      <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
@@ -1285,7 +1280,7 @@
       <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="F42">
+      <c r="C42">
         <v>1</v>
       </c>
     </row>
@@ -1302,11 +1297,11 @@
         <v>50</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
+      <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -1317,10 +1312,10 @@
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -1329,7 +1324,7 @@
       <c r="A46" t="s">
         <v>52</v>
       </c>
-      <c r="D46">
+      <c r="C46">
         <v>1</v>
       </c>
     </row>
@@ -1337,7 +1332,7 @@
       <c r="A47" t="s">
         <v>53</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>1</v>
       </c>
     </row>
@@ -1347,10 +1342,10 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="2">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -1360,14 +1355,16 @@
         <v>55</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
       <c r="D49" s="2"/>
-      <c r="E49" s="2">
-        <v>1</v>
-      </c>
+      <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="H49" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -1376,9 +1373,6 @@
       <c r="C50">
         <v>1</v>
       </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1393,13 +1387,13 @@
         <v>58</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="2">
-        <v>1</v>
-      </c>
+      <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="G52" s="2">
+        <v>1</v>
+      </c>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1407,13 +1401,13 @@
         <v>59</v>
       </c>
       <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="2">
-        <v>1</v>
-      </c>
+      <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1428,7 +1422,7 @@
       <c r="A55" t="s">
         <v>61</v>
       </c>
-      <c r="C55">
+      <c r="G55">
         <v>1</v>
       </c>
     </row>
@@ -1437,13 +1431,13 @@
         <v>62</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="2">
-        <v>1</v>
-      </c>
+      <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1464,7 +1458,7 @@
       <c r="A58" t="s">
         <v>64</v>
       </c>
-      <c r="C58">
+      <c r="F58">
         <v>1</v>
       </c>
     </row>
@@ -1472,6 +1466,9 @@
       <c r="A59" t="s">
         <v>65</v>
       </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
       <c r="F59">
         <v>1</v>
       </c>
@@ -1486,9 +1483,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="2"/>
-      <c r="F60" s="2">
-        <v>1</v>
-      </c>
+      <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
@@ -1497,10 +1492,10 @@
         <v>67</v>
       </c>
       <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2">
-        <v>1</v>
-      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -1518,7 +1513,7 @@
       <c r="A63" t="s">
         <v>69</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <v>1</v>
       </c>
     </row>
@@ -1527,10 +1522,10 @@
         <v>70</v>
       </c>
       <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2">
-        <v>1</v>
-      </c>
+      <c r="C64" s="2">
+        <v>1</v>
+      </c>
+      <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -1572,10 +1567,10 @@
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2">
-        <v>1</v>
-      </c>
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -1585,10 +1580,10 @@
         <v>75</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
+      <c r="C69" s="2">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -1615,11 +1610,11 @@
         <v>78</v>
       </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="2">
-        <v>1</v>
-      </c>
+      <c r="C72" s="2"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
+      <c r="E72" s="2">
+        <v>1</v>
+      </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -1630,10 +1625,10 @@
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2">
-        <v>1</v>
-      </c>
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -1642,7 +1637,7 @@
       <c r="A74" t="s">
         <v>80</v>
       </c>
-      <c r="D74">
+      <c r="C74">
         <v>1</v>
       </c>
     </row>
@@ -1694,7 +1689,7 @@
       <c r="A79" t="s">
         <v>85</v>
       </c>
-      <c r="C79">
+      <c r="E79">
         <v>1</v>
       </c>
     </row>
@@ -1703,11 +1698,11 @@
         <v>86</v>
       </c>
       <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
+      <c r="C80" s="2">
+        <v>1</v>
+      </c>
       <c r="D80" s="2"/>
-      <c r="E80" s="2">
-        <v>1</v>
-      </c>
+      <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -1717,11 +1712,11 @@
         <v>87</v>
       </c>
       <c r="B81" s="2"/>
-      <c r="C81" s="2">
-        <v>1</v>
-      </c>
+      <c r="C81" s="2"/>
       <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="E81" s="2">
+        <v>1</v>
+      </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -1738,7 +1733,7 @@
       <c r="A83" t="s">
         <v>89</v>
       </c>
-      <c r="E83">
+      <c r="C83">
         <v>1</v>
       </c>
     </row>
@@ -1747,13 +1742,13 @@
         <v>90</v>
       </c>
       <c r="B84" s="2"/>
-      <c r="C84" s="2">
-        <v>1</v>
-      </c>
+      <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
+      <c r="G84" s="2">
+        <v>1</v>
+      </c>
       <c r="H84" s="2"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -1761,13 +1756,15 @@
         <v>91</v>
       </c>
       <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+      <c r="C85" s="2">
+        <v>1</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="2">
-        <v>1</v>
-      </c>
+      <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -1775,9 +1772,6 @@
         <v>92</v>
       </c>
       <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86">
         <v>1</v>
       </c>
     </row>
@@ -1821,7 +1815,7 @@
       <c r="A90" t="s">
         <v>96</v>
       </c>
-      <c r="C90">
+      <c r="D90">
         <v>1</v>
       </c>
     </row>
@@ -1829,6 +1823,9 @@
       <c r="A91" t="s">
         <v>97</v>
       </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
       <c r="D91">
         <v>1</v>
       </c>
@@ -1841,9 +1838,7 @@
       <c r="C92" s="2">
         <v>1</v>
       </c>
-      <c r="D92" s="2">
-        <v>1</v>
-      </c>
+      <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -1911,7 +1906,7 @@
       <c r="A98" t="s">
         <v>104</v>
       </c>
-      <c r="C98">
+      <c r="E98">
         <v>1</v>
       </c>
     </row>
@@ -1919,7 +1914,7 @@
       <c r="A99" t="s">
         <v>105</v>
       </c>
-      <c r="E99">
+      <c r="C99">
         <v>1</v>
       </c>
     </row>
@@ -1928,12 +1923,14 @@
         <v>106</v>
       </c>
       <c r="B100" s="2"/>
-      <c r="C100" s="2">
-        <v>1</v>
-      </c>
-      <c r="D100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2">
+        <v>1</v>
+      </c>
       <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
+      <c r="F100" s="2">
+        <v>1</v>
+      </c>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -1941,15 +1938,13 @@
       <c r="A101" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B101" s="2"/>
+      <c r="B101" s="2">
+        <v>1</v>
+      </c>
       <c r="C101" s="2"/>
-      <c r="D101" s="2">
-        <v>1</v>
-      </c>
+      <c r="D101" s="2"/>
       <c r="E101" s="2"/>
-      <c r="F101" s="2">
-        <v>1</v>
-      </c>
+      <c r="F101" s="2"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
     </row>
@@ -1957,7 +1952,7 @@
       <c r="A102" t="s">
         <v>108</v>
       </c>
-      <c r="B102">
+      <c r="C102">
         <v>1</v>
       </c>
     </row>
@@ -1965,7 +1960,7 @@
       <c r="A103" t="s">
         <v>109</v>
       </c>
-      <c r="C103">
+      <c r="D103">
         <v>1</v>
       </c>
     </row>
@@ -1974,10 +1969,10 @@
         <v>110</v>
       </c>
       <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2">
-        <v>1</v>
-      </c>
+      <c r="C104" s="2">
+        <v>1</v>
+      </c>
+      <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
@@ -2009,7 +2004,7 @@
       <c r="A107" t="s">
         <v>113</v>
       </c>
-      <c r="C107">
+      <c r="D107">
         <v>1</v>
       </c>
     </row>
@@ -2018,10 +2013,10 @@
         <v>114</v>
       </c>
       <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2">
-        <v>1</v>
-      </c>
+      <c r="C108" s="2">
+        <v>1</v>
+      </c>
+      <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
@@ -2048,6 +2043,9 @@
       <c r="C110">
         <v>1</v>
       </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
@@ -2065,9 +2063,7 @@
       <c r="C112" s="2">
         <v>1</v>
       </c>
-      <c r="D112" s="2">
-        <v>1</v>
-      </c>
+      <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
@@ -2078,30 +2074,14 @@
         <v>119</v>
       </c>
       <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
+      <c r="C113" s="2">
+        <v>1</v>
+      </c>
       <c r="D113" s="2"/>
-      <c r="E113" s="2">
-        <v>1</v>
-      </c>
+      <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>120</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>121</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>

</xml_diff>

<commit_message>
Docu update for Rel 9.00 RC2
</commit_message>
<xml_diff>
--- a/Images/Countries.xlsx
+++ b/Images/Countries.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Country name</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Honduras</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
   <si>
     <t>Ireland</t>
@@ -759,7 +762,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0000-0000-0000-000000000000}">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H110"/>
   <!-- B4P: Example: A1:Z9 -->
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1" showGridLines="0">
@@ -1350,7 +1353,9 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="H49" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -1364,7 +1369,7 @@
       <c r="A51" t="s">
         <v>57</v>
       </c>
-      <c r="G51">
+      <c r="C51">
         <v>1</v>
       </c>
     </row>
@@ -1373,13 +1378,13 @@
         <v>58</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="2">
-        <v>1</v>
-      </c>
+      <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="G52" s="2">
+        <v>1</v>
+      </c>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1400,7 +1405,7 @@
       <c r="A54" t="s">
         <v>60</v>
       </c>
-      <c r="G54">
+      <c r="C54">
         <v>1</v>
       </c>
     </row>
@@ -1408,7 +1413,7 @@
       <c r="A55" t="s">
         <v>61</v>
       </c>
-      <c r="C55">
+      <c r="G55">
         <v>1</v>
       </c>
     </row>
@@ -1431,12 +1436,12 @@
         <v>63</v>
       </c>
       <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="2">
-        <v>1</v>
-      </c>
+      <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
@@ -1444,9 +1449,6 @@
       <c r="A58" t="s">
         <v>64</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
       <c r="F58">
         <v>1</v>
       </c>
@@ -1458,16 +1460,19 @@
       <c r="D59">
         <v>1</v>
       </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B60" s="2"/>
-      <c r="C60" s="2">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -1478,10 +1483,10 @@
         <v>67</v>
       </c>
       <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2">
-        <v>1</v>
-      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -1491,7 +1496,7 @@
       <c r="A62" t="s">
         <v>68</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <v>1</v>
       </c>
     </row>
@@ -1535,7 +1540,7 @@
       <c r="A66" t="s">
         <v>72</v>
       </c>
-      <c r="D66">
+      <c r="C66">
         <v>1</v>
       </c>
     </row>
@@ -1543,7 +1548,7 @@
       <c r="A67" t="s">
         <v>73</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <v>1</v>
       </c>
     </row>
@@ -1566,11 +1571,11 @@
         <v>75</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="C69" s="2">
+        <v>1</v>
+      </c>
       <c r="D69" s="2"/>
-      <c r="E69" s="2">
-        <v>1</v>
-      </c>
+      <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -1579,7 +1584,7 @@
       <c r="A70" t="s">
         <v>76</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>1</v>
       </c>
     </row>
@@ -1587,7 +1592,7 @@
       <c r="A71" t="s">
         <v>77</v>
       </c>
-      <c r="C71">
+      <c r="D71">
         <v>1</v>
       </c>
     </row>
@@ -1640,11 +1645,11 @@
         <v>82</v>
       </c>
       <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
       <c r="D76" s="2"/>
-      <c r="E76" s="2">
-        <v>1</v>
-      </c>
+      <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -1654,11 +1659,11 @@
         <v>83</v>
       </c>
       <c r="B77" s="2"/>
-      <c r="C77" s="2">
-        <v>1</v>
-      </c>
+      <c r="C77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
+      <c r="E77" s="2">
+        <v>1</v>
+      </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -1667,7 +1672,7 @@
       <c r="A78" t="s">
         <v>84</v>
       </c>
-      <c r="E78">
+      <c r="C78">
         <v>1</v>
       </c>
     </row>
@@ -1684,11 +1689,11 @@
         <v>86</v>
       </c>
       <c r="B80" s="2"/>
-      <c r="C80" s="2">
-        <v>1</v>
-      </c>
+      <c r="C80" s="2"/>
       <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+      <c r="E80" s="2">
+        <v>1</v>
+      </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -1698,23 +1703,20 @@
         <v>87</v>
       </c>
       <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
+      <c r="C81" s="2">
+        <v>1</v>
+      </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="2">
-        <v>1</v>
-      </c>
+      <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-      <c r="D82">
+      <c r="G82">
         <v>1</v>
       </c>
     </row>
@@ -1723,6 +1725,9 @@
         <v>89</v>
       </c>
       <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
         <v>1</v>
       </c>
     </row>
@@ -1766,7 +1771,7 @@
       <c r="A87" t="s">
         <v>93</v>
       </c>
-      <c r="D87">
+      <c r="C87">
         <v>1</v>
       </c>
     </row>
@@ -1775,9 +1780,7 @@
         <v>94</v>
       </c>
       <c r="B88" s="2"/>
-      <c r="C88" s="2">
-        <v>1</v>
-      </c>
+      <c r="C88" s="2"/>
       <c r="D88" s="2">
         <v>1</v>
       </c>
@@ -1794,7 +1797,9 @@
       <c r="C89" s="2">
         <v>1</v>
       </c>
-      <c r="D89" s="2"/>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -1856,7 +1861,7 @@
       <c r="A95" t="s">
         <v>101</v>
       </c>
-      <c r="E95">
+      <c r="C95">
         <v>1</v>
       </c>
     </row>
@@ -1865,11 +1870,11 @@
         <v>102</v>
       </c>
       <c r="B96" s="2"/>
-      <c r="C96" s="2">
-        <v>1</v>
-      </c>
+      <c r="C96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
+      <c r="E96" s="2">
+        <v>1</v>
+      </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -1879,14 +1884,12 @@
         <v>103</v>
       </c>
       <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2">
-        <v>1</v>
-      </c>
+      <c r="C97" s="2">
+        <v>1</v>
+      </c>
+      <c r="D97" s="2"/>
       <c r="E97" s="2"/>
-      <c r="F97" s="2">
-        <v>1</v>
-      </c>
+      <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
@@ -1894,7 +1897,10 @@
       <c r="A98" t="s">
         <v>104</v>
       </c>
-      <c r="C98">
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="F98">
         <v>1</v>
       </c>
     </row>
@@ -1902,7 +1908,7 @@
       <c r="A99" t="s">
         <v>105</v>
       </c>
-      <c r="D99">
+      <c r="C99">
         <v>1</v>
       </c>
     </row>
@@ -1911,10 +1917,10 @@
         <v>106</v>
       </c>
       <c r="B100" s="2"/>
-      <c r="C100" s="2">
-        <v>1</v>
-      </c>
-      <c r="D100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2">
+        <v>1</v>
+      </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -1946,7 +1952,7 @@
       <c r="A103" t="s">
         <v>109</v>
       </c>
-      <c r="D103">
+      <c r="C103">
         <v>1</v>
       </c>
     </row>
@@ -1955,10 +1961,10 @@
         <v>110</v>
       </c>
       <c r="B104" s="2"/>
-      <c r="C104" s="2">
-        <v>1</v>
-      </c>
-      <c r="D104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2">
+        <v>1</v>
+      </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
@@ -1985,15 +1991,15 @@
       <c r="C106">
         <v>1</v>
       </c>
-      <c r="D106">
-        <v>1</v>
-      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>113</v>
       </c>
-      <c r="E107">
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
         <v>1</v>
       </c>
     </row>
@@ -2002,11 +2008,11 @@
         <v>114</v>
       </c>
       <c r="B108" s="2"/>
-      <c r="C108" s="2">
-        <v>1</v>
-      </c>
+      <c r="C108" s="2"/>
       <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
+      <c r="E108" s="2">
+        <v>1</v>
+      </c>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -2024,6 +2030,14 @@
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>116</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>

</xml_diff>